<commit_message>
zmiana w dodatkach centa i podsumowanie
</commit_message>
<xml_diff>
--- a/WYCENY.xlsx
+++ b/WYCENY.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\48534\Desktop\aluko-app2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFDADFB8-F12B-40C3-A379-6F62485F4C58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B47BC6-449A-4A33-B380-EC2344DC3466}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-30" windowWidth="29040" windowHeight="15720" tabRatio="739" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="34">
   <si>
     <t>HS 2 Skrzydla</t>
   </si>
@@ -111,6 +111,30 @@
   </si>
   <si>
     <t>HS</t>
+  </si>
+  <si>
+    <t>HS kontaktron 1 naskrzydło czyli 2x 312 zł</t>
+  </si>
+  <si>
+    <t>HS okucie Silent Close 1 naskrzydło czyli 2 x 1298 zł</t>
+  </si>
+  <si>
+    <t>HS Klamka dwustronna z wkładką obustronną na skrzydło czyli 2x519 zł</t>
+  </si>
+  <si>
+    <t>HS Wkładka jednostronna na 1 skrzydło czyli 2x157 zł</t>
+  </si>
+  <si>
+    <t>Kontaktron MC250 1 naskrzydło czyli 2x 121 zł</t>
+  </si>
+  <si>
+    <t>Systemowy kontaktron z kontrolą ryglowania 1 naskrzydło czyli 2x 573 zł</t>
+  </si>
+  <si>
+    <t>Mikrowentylacja ROTO 1 naskrzydło czyli 2x 194 zł</t>
+  </si>
+  <si>
+    <t>Zatzask balkonowy z pochwytem 1 naskrzydło czyli 2x 119 zł</t>
   </si>
 </sst>
 </file>
@@ -987,7 +1011,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>45342</xdr:colOff>
+      <xdr:colOff>48517</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>38992</xdr:rowOff>
     </xdr:to>
@@ -1535,8 +1559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2292162-4499-4263-B7E0-1999D5CFEB55}">
   <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20:M24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1930,7 +1954,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="20" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" s="14" t="s">
         <v>8</v>
       </c>
@@ -1938,7 +1962,7 @@
         <v>1298</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="30" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="14" t="s">
         <v>9</v>
       </c>
@@ -1946,7 +1970,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="20" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="14" t="s">
         <v>10</v>
       </c>
@@ -1969,14 +1993,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20:M24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="28.1796875" customWidth="1"/>
-    <col min="2" max="2" width="10.453125" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
     <col min="4" max="10" width="12.26953125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16.54296875" bestFit="1" customWidth="1"/>
@@ -2357,36 +2381,36 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" ht="20" x14ac:dyDescent="0.35">
       <c r="A31" s="14" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="B31" s="15">
-        <v>312</v>
+        <v>624</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="20" x14ac:dyDescent="0.35">
       <c r="A32" s="14" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="B32" s="15">
-        <v>1298</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="40" x14ac:dyDescent="0.35">
+        <v>2596</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="30" x14ac:dyDescent="0.35">
       <c r="A33" s="14" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="B33" s="15">
-        <v>519</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="20" x14ac:dyDescent="0.35">
       <c r="A34" s="14" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="B34" s="15">
-        <v>157</v>
+        <v>314</v>
       </c>
     </row>
   </sheetData>
@@ -2405,7 +2429,7 @@
   <dimension ref="A1:Q34"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="T33" sqref="T33"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3439,7 +3463,7 @@
       <c r="P30" s="25"/>
       <c r="Q30" s="15"/>
     </row>
-    <row r="31" spans="1:17" ht="20" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" s="25" t="s">
         <v>12</v>
       </c>
@@ -3449,7 +3473,7 @@
       <c r="P31" s="25"/>
       <c r="Q31" s="15"/>
     </row>
-    <row r="32" spans="1:17" ht="40" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:17" ht="20" x14ac:dyDescent="0.35">
       <c r="A32" s="25" t="s">
         <v>13</v>
       </c>
@@ -3459,7 +3483,7 @@
       <c r="P32" s="25"/>
       <c r="Q32" s="15"/>
     </row>
-    <row r="33" spans="1:2" ht="20" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="25" t="s">
         <v>14</v>
       </c>
@@ -3467,7 +3491,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="30" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="25" t="s">
         <v>15</v>
       </c>
@@ -3490,8 +3514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3132394-8E5A-4DE4-B592-9A731C6D40F1}">
   <dimension ref="A1:Q34"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="M31" sqref="M31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4418,7 +4442,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="20" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" s="25" t="s">
         <v>12</v>
       </c>
@@ -4426,7 +4450,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="32" spans="1:17" ht="40" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:17" ht="20" x14ac:dyDescent="0.35">
       <c r="A32" s="25" t="s">
         <v>13</v>
       </c>
@@ -4434,7 +4458,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="20" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="25" t="s">
         <v>14</v>
       </c>
@@ -4442,13 +4466,9 @@
         <v>194</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="30" x14ac:dyDescent="0.35">
-      <c r="A34" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="B34" s="15">
-        <v>119</v>
-      </c>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" s="25"/>
+      <c r="B34" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4466,13 +4486,13 @@
   <dimension ref="A1:Y34"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="T32" sqref="T32"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="40.54296875" customWidth="1"/>
-    <col min="2" max="2" width="10.54296875" customWidth="1"/>
+    <col min="2" max="2" width="13.1796875" customWidth="1"/>
     <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
     <col min="4" max="20" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="21" max="22" width="12.26953125" bestFit="1" customWidth="1"/>
@@ -6109,40 +6129,40 @@
       <c r="X30" s="25"/>
       <c r="Y30" s="15"/>
     </row>
-    <row r="31" spans="1:25" ht="20" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A31" s="25" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="B31" s="15">
-        <v>121</v>
+        <v>242</v>
       </c>
       <c r="X31" s="25"/>
       <c r="Y31" s="15"/>
     </row>
-    <row r="32" spans="1:25" ht="40" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:25" ht="20" x14ac:dyDescent="0.35">
       <c r="A32" s="25" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="B32" s="15">
-        <v>573</v>
+        <v>1146</v>
       </c>
       <c r="X32" s="25"/>
       <c r="Y32" s="15"/>
     </row>
-    <row r="33" spans="1:2" ht="20" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="25" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="B33" s="15">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="30" x14ac:dyDescent="0.35">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="20" x14ac:dyDescent="0.35">
       <c r="A34" s="25" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="B34" s="15">
-        <v>119</v>
+        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -6161,7 +6181,7 @@
   <dimension ref="A1:Y34"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="T33" sqref="T33"/>
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7615,41 +7635,37 @@
       <c r="X30" s="25"/>
       <c r="Y30" s="15"/>
     </row>
-    <row r="31" spans="1:25" ht="20" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A31" s="25" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="B31" s="15">
-        <v>121</v>
+        <v>242</v>
       </c>
       <c r="X31" s="25"/>
       <c r="Y31" s="15"/>
     </row>
-    <row r="32" spans="1:25" ht="40" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:25" ht="20" x14ac:dyDescent="0.35">
       <c r="A32" s="25" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="B32" s="15">
-        <v>573</v>
+        <v>1146</v>
       </c>
       <c r="X32" s="25"/>
       <c r="Y32" s="15"/>
     </row>
-    <row r="33" spans="1:2" ht="20" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="25" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="B33" s="15">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="30" x14ac:dyDescent="0.35">
-      <c r="A34" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="B34" s="15">
-        <v>119</v>
-      </c>
+        <v>388</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" s="25"/>
+      <c r="B34" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -7666,8 +7682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5378C79B-0E42-44A4-AB1B-56918D9B4ECC}">
   <dimension ref="A1:Y34"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="U31" sqref="U31"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9117,17 +9133,17 @@
       <c r="X30" s="25"/>
       <c r="Y30" s="15"/>
     </row>
-    <row r="31" spans="1:25" ht="20" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A31" s="25" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="B31" s="15">
-        <v>121</v>
+        <v>242</v>
       </c>
       <c r="X31" s="25"/>
       <c r="Y31" s="15"/>
     </row>
-    <row r="32" spans="1:25" ht="40" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A32" s="25" t="s">
         <v>13</v>
       </c>
@@ -9137,7 +9153,7 @@
       <c r="X32" s="25"/>
       <c r="Y32" s="15"/>
     </row>
-    <row r="33" spans="1:2" ht="20" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="25" t="s">
         <v>14</v>
       </c>
@@ -9145,13 +9161,9 @@
         <v>194</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="30" x14ac:dyDescent="0.35">
-      <c r="A34" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="B34" s="15">
-        <v>119</v>
-      </c>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" s="25"/>
+      <c r="B34" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -9168,8 +9180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1F75182-FF93-4610-9DD1-45EF747A5A10}">
   <dimension ref="A1:Y34"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10823,10 +10835,10 @@
     </row>
     <row r="31" spans="1:25" ht="20" x14ac:dyDescent="0.35">
       <c r="A31" s="25" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="B31" s="15">
-        <v>121</v>
+        <v>242</v>
       </c>
       <c r="X31" s="25" t="s">
         <v>14</v>
@@ -10835,7 +10847,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="32" spans="1:25" ht="40" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:25" ht="20" x14ac:dyDescent="0.35">
       <c r="A32" s="25" t="s">
         <v>13</v>
       </c>
@@ -10849,7 +10861,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="20" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="25" t="s">
         <v>14</v>
       </c>
@@ -10857,7 +10869,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="30" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="25" t="s">
         <v>16</v>
       </c>
@@ -10880,7 +10892,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D253740-FE97-4FFB-B698-DA3D3419EA93}">
   <dimension ref="A1:AD29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>

</xml_diff>